<commit_message>
Total Survey Station Estimations
Worked on Code to estimate how many stations possible for upcoming survey.  Using DY19-05 Station locations:
'SRT data' mirrors the "survey run time spreadsheets" used on all FOCI surveys
Code to Filter out stations needs to be done
'ShipsLog' gives a final datetime listing of station operations
</commit_message>
<xml_diff>
--- a/Data/2023-02-10_JFL_Final_StationRunTime_WO21_01_For R.xlsx
+++ b/Data/2023-02-10_JFL_Final_StationRunTime_WO21_01_For R.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Lamb\Field Work\FW 2023\DY23-07\Survey Station Run Time R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.f.lamb\Work\GitHub\Survey_Station_Selection\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Est. Transit times'!$A$1:$A$234</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7705,6 +7705,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A161:E161"/>
     <mergeCell ref="A82:E82"/>
     <mergeCell ref="A91:E91"/>
@@ -7714,15 +7723,6 @@
     <mergeCell ref="A128:E128"/>
     <mergeCell ref="A138:E138"/>
     <mergeCell ref="A148:E148"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="A73:E73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A39:E39"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7735,7 +7735,7 @@
   <dimension ref="A1:U234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
@@ -8246,15 +8246,15 @@
         <v>10</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1.8665801302237139</v>
       </c>
       <c r="M8" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" ca="1" si="6"/>
         <v>44325.485740324482</v>
       </c>
       <c r="N8" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" ca="1" si="7"/>
         <v>44325.513240324479</v>
       </c>
       <c r="O8" s="8">
@@ -8262,23 +8262,23 @@
         <v>58.957999999999998</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="9"/>
-        <v>-151.119</v>
+        <f ca="1">L8=E8</f>
+        <v>0</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="10"/>
         <v>1.0290112203908168</v>
       </c>
       <c r="R8" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" ca="1" si="11"/>
         <v>-2.6375241123213109</v>
       </c>
       <c r="S8" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" ca="1" si="12"/>
         <v>-7.1034900556172786E-3</v>
       </c>
       <c r="T8" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" ca="1" si="13"/>
         <v>18.665801302237139</v>
       </c>
     </row>
@@ -8314,7 +8314,7 @@
         <v>10</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1.4111069106650018</v>
       </c>
       <c r="M9" s="15">
@@ -8341,11 +8341,11 @@
         <v>-2.6378382715866695</v>
       </c>
       <c r="S9" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" ca="1" si="12"/>
         <v>-3.141592653586045E-4</v>
       </c>
       <c r="T9" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" ca="1" si="13"/>
         <v>14.111069106650019</v>
       </c>
     </row>

</xml_diff>